<commit_message>
Add excel iterative calculation
</commit_message>
<xml_diff>
--- a/tests/fixtures/circular.xlsx
+++ b/tests/fixtures/circular.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpenton/Development/pycel/tests/fixtures/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94C26BD-28F2-0544-AB00-04D937B6513E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{3AB6E7BF-3554-764B-A396-D7D971122863}"/>
+    <workbookView xWindow="375" yWindow="465" windowWidth="28035" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725" iterate="1" iterateCount="10000" iterateDelta="0.01"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -29,9 +23,16 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="175" formatCode="0.00000000"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,9 +69,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -132,7 +134,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -184,7 +186,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -378,43 +380,75 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEEB6FAD-BA51-724F-AAAB-E5F546F6B845}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="16.625" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B1">
-        <f ca="1">B3-B2</f>
-        <v>-4.3269140487790506E-77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
+      <c r="B1" s="2">
+        <f>B3-B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>0.2</v>
       </c>
-      <c r="B2">
-        <f ca="1">A2*B1</f>
-        <v>-8.6538280975581008E-78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B3">
+      <c r="B2" s="2">
+        <f>IF(B3=0, 0, A2*B1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <f>B6</f>
+        <v>50</v>
+      </c>
+      <c r="B6" s="2">
+        <f>IF(B3=0, A5,IF(A6&lt;0,A5, A6-B5))</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" s="2">
+        <f>B1-B6</f>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" s="2">
+        <f>IF(B3=0, 0, B10+0.001)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>